<commit_message>
progress on execute; handful of decode connections
</commit_message>
<xml_diff>
--- a/Truth Table.xlsx
+++ b/Truth Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22000" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22000" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
   <si>
     <t>Op</t>
   </si>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:Q15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1603,8 +1603,8 @@
       <c r="S20">
         <v>0</v>
       </c>
-      <c r="T20" t="s">
-        <v>4</v>
+      <c r="T20">
+        <v>1</v>
       </c>
       <c r="U20">
         <v>1</v>
@@ -1668,8 +1668,8 @@
       <c r="S21">
         <v>0</v>
       </c>
-      <c r="T21" t="s">
-        <v>4</v>
+      <c r="T21">
+        <v>1</v>
       </c>
       <c r="U21">
         <v>1</v>
@@ -1733,8 +1733,8 @@
       <c r="S22">
         <v>0</v>
       </c>
-      <c r="T22" t="s">
-        <v>4</v>
+      <c r="T22">
+        <v>1</v>
       </c>
       <c r="U22">
         <v>1</v>
@@ -1798,8 +1798,8 @@
       <c r="S23">
         <v>0</v>
       </c>
-      <c r="T23" t="s">
-        <v>4</v>
+      <c r="T23">
+        <v>0</v>
       </c>
       <c r="U23">
         <v>1</v>
@@ -1863,8 +1863,8 @@
       <c r="S24">
         <v>0</v>
       </c>
-      <c r="T24" t="s">
-        <v>4</v>
+      <c r="T24">
+        <v>0</v>
       </c>
       <c r="U24">
         <v>1</v>
@@ -1928,8 +1928,8 @@
       <c r="S25">
         <v>0</v>
       </c>
-      <c r="T25" t="s">
-        <v>4</v>
+      <c r="T25">
+        <v>0</v>
       </c>
       <c r="U25">
         <v>1</v>

</xml_diff>